<commit_message>
Added Expansion completely, Filling to stands, added more shopitem sprites, added coloring of filling state of stands, Next: Add more shopitems, add shopitem levels, add shoptime story where they come from and upgrades to get more shopitems.
</commit_message>
<xml_diff>
--- a/GuildManager2d/CSV/shop_item.xlsx
+++ b/GuildManager2d/CSV/shop_item.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\GodotProjects\Games\GuildManagerFolder\GuildManager2d\CSV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\MedievalStoreManager\GuildManager2d\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2A59F7-6106-4757-9382-802B9AE66CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F1AD31-5528-46B7-BB24-494A70604DBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25490" yWindow="3460" windowWidth="19420" windowHeight="10560" xr2:uid="{6613D835-19EA-40EE-98A1-1D2837994A45}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="10305" xr2:uid="{6613D835-19EA-40EE-98A1-1D2837994A45}"/>
   </bookViews>
   <sheets>
     <sheet name="shop_item" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="58">
   <si>
     <t>id</t>
   </si>
@@ -179,6 +179,21 @@
   </si>
   <si>
     <t>market_value</t>
+  </si>
+  <si>
+    <t>average_color</t>
+  </si>
+  <si>
+    <t>160,104,73</t>
+  </si>
+  <si>
+    <t>220,55,70</t>
+  </si>
+  <si>
+    <t>105,76,77</t>
+  </si>
+  <si>
+    <t>243,131,27</t>
   </si>
 </sst>
 </file>
@@ -1055,7 +1070,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1068,6 +1083,7 @@
     <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.7109375" customWidth="1"/>
     <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1104,6 +1120,9 @@
       <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="L1" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="2" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -1139,6 +1158,9 @@
       </c>
       <c r="K2">
         <v>50</v>
+      </c>
+      <c r="L2" t="s">
+        <v>54</v>
       </c>
       <c r="M2" s="1"/>
     </row>
@@ -1178,6 +1200,9 @@
       <c r="K3">
         <v>30</v>
       </c>
+      <c r="L3" t="s">
+        <v>56</v>
+      </c>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1216,6 +1241,9 @@
       <c r="K4">
         <v>100</v>
       </c>
+      <c r="L4" t="s">
+        <v>55</v>
+      </c>
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1254,6 +1282,9 @@
       <c r="K5">
         <v>20</v>
       </c>
+      <c r="L5" t="s">
+        <v>57</v>
+      </c>
       <c r="M5" s="1"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>